<commit_message>
Fixed data collector and track xodr
</commit_message>
<xml_diff>
--- a/ros_bridge/src/carla_data/lap_data3.xlsx
+++ b/ros_bridge/src/carla_data/lap_data3.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:S10"/>
+  <dimension ref="A1:S16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1097,6 +1097,384 @@
         </is>
       </c>
     </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>2</v>
+      </c>
+      <c r="B11" t="n">
+        <v>11.06016896578102</v>
+      </c>
+      <c r="C11" t="n">
+        <v>0.002294959556662829</v>
+      </c>
+      <c r="D11" t="n">
+        <v>473.9336707852781</v>
+      </c>
+      <c r="E11" t="n">
+        <v>113.4843755593174</v>
+      </c>
+      <c r="F11" t="n">
+        <v>8.901275970041752</v>
+      </c>
+      <c r="G11" t="n">
+        <v>0.3273026943206787</v>
+      </c>
+      <c r="H11" t="n">
+        <v>-1.404465198516846</v>
+      </c>
+      <c r="I11" t="n">
+        <v>10.03396511077881</v>
+      </c>
+      <c r="J11" t="n">
+        <v>-0.0141261350363493</v>
+      </c>
+      <c r="K11" t="n">
+        <v>0.00764760747551918</v>
+      </c>
+      <c r="L11" t="n">
+        <v>0.4508436620235443</v>
+      </c>
+      <c r="M11" t="n">
+        <v>32.07910814767075</v>
+      </c>
+      <c r="N11" t="n">
+        <v>34.78034595374852</v>
+      </c>
+      <c r="O11" t="n">
+        <v>1.992981791496277</v>
+      </c>
+      <c r="P11" t="n">
+        <v>3.579217070074993</v>
+      </c>
+      <c r="Q11" t="n">
+        <v>82.570647411</v>
+      </c>
+      <c r="R11" t="inlineStr">
+        <is>
+          <t>2025-03-13 17:36:51</t>
+        </is>
+      </c>
+      <c r="S11" t="inlineStr">
+        <is>
+          <t>vehicle.audi.a2</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>3</v>
+      </c>
+      <c r="B12" t="n">
+        <v>10.90638750309475</v>
+      </c>
+      <c r="C12" t="n">
+        <v>0.01190849502506625</v>
+      </c>
+      <c r="D12" t="n">
+        <v>435.3277809685096</v>
+      </c>
+      <c r="E12" t="n">
+        <v>110.8955901527079</v>
+      </c>
+      <c r="F12" t="n">
+        <v>7.352978865616024</v>
+      </c>
+      <c r="G12" t="n">
+        <v>4.297463417053223</v>
+      </c>
+      <c r="H12" t="n">
+        <v>-6.678197383880615</v>
+      </c>
+      <c r="I12" t="n">
+        <v>9.789709091186523</v>
+      </c>
+      <c r="J12" t="n">
+        <v>-0.001004496356472373</v>
+      </c>
+      <c r="K12" t="n">
+        <v>0.0009123191703110933</v>
+      </c>
+      <c r="L12" t="n">
+        <v>-0.4723412394523621</v>
+      </c>
+      <c r="M12" t="n">
+        <v>32.07943472061575</v>
+      </c>
+      <c r="N12" t="n">
+        <v>34.78054325839844</v>
+      </c>
+      <c r="O12" t="n">
+        <v>2.038751363754272</v>
+      </c>
+      <c r="P12" t="n">
+        <v>2.993654337598892</v>
+      </c>
+      <c r="Q12" t="n">
+        <v>78.516544149</v>
+      </c>
+      <c r="R12" t="inlineStr">
+        <is>
+          <t>2025-03-13 17:38:09</t>
+        </is>
+      </c>
+      <c r="S12" t="inlineStr">
+        <is>
+          <t>vehicle.citroen.c3</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>1</v>
+      </c>
+      <c r="B13" t="n">
+        <v>0.01124353238297381</v>
+      </c>
+      <c r="C13" t="n">
+        <v>2.683445229236883e-08</v>
+      </c>
+      <c r="D13" t="n">
+        <v>7.650000214576721</v>
+      </c>
+      <c r="E13" t="n">
+        <v>0.9441008344292641</v>
+      </c>
+      <c r="F13" t="n">
+        <v>0</v>
+      </c>
+      <c r="G13" t="n">
+        <v>1.449541449546814</v>
+      </c>
+      <c r="H13" t="n">
+        <v>-0.004217132460325956</v>
+      </c>
+      <c r="I13" t="n">
+        <v>7.848243236541748</v>
+      </c>
+      <c r="J13" t="n">
+        <v>-1.148816681961762e-05</v>
+      </c>
+      <c r="K13" t="n">
+        <v>0.0007947385311126709</v>
+      </c>
+      <c r="L13" t="n">
+        <v>1.177044737232791e-06</v>
+      </c>
+      <c r="M13" t="n">
+        <v>32.08033253413927</v>
+      </c>
+      <c r="N13" t="n">
+        <v>34.78079790662085</v>
+      </c>
+      <c r="O13" t="n">
+        <v>1.97679328918457</v>
+      </c>
+      <c r="P13" t="n">
+        <v>0.0005727527130562226</v>
+      </c>
+      <c r="Q13" t="n">
+        <v>1.002568905</v>
+      </c>
+      <c r="R13" t="inlineStr">
+        <is>
+          <t>2025-03-13 17:51:05</t>
+        </is>
+      </c>
+      <c r="S13" t="inlineStr">
+        <is>
+          <t>vehicle.audi.a2</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>1</v>
+      </c>
+      <c r="B14" t="n">
+        <v>0.01292331612844646</v>
+      </c>
+      <c r="C14" t="n">
+        <v>2.549362268908855e-08</v>
+      </c>
+      <c r="D14" t="n">
+        <v>7.650000214576721</v>
+      </c>
+      <c r="E14" t="n">
+        <v>0.9255037233233452</v>
+      </c>
+      <c r="F14" t="n">
+        <v>0</v>
+      </c>
+      <c r="G14" t="n">
+        <v>0.3324514031410217</v>
+      </c>
+      <c r="H14" t="n">
+        <v>0.159079298377037</v>
+      </c>
+      <c r="I14" t="n">
+        <v>9.329581260681152</v>
+      </c>
+      <c r="J14" t="n">
+        <v>-5.366017830965575e-06</v>
+      </c>
+      <c r="K14" t="n">
+        <v>0.001075407606549561</v>
+      </c>
+      <c r="L14" t="n">
+        <v>1.541746769362362e-06</v>
+      </c>
+      <c r="M14" t="n">
+        <v>32.08033253414786</v>
+      </c>
+      <c r="N14" t="n">
+        <v>34.78079790540754</v>
+      </c>
+      <c r="O14" t="n">
+        <v>1.964659690856934</v>
+      </c>
+      <c r="P14" t="n">
+        <v>0.0009882330150246383</v>
+      </c>
+      <c r="Q14" t="n">
+        <v>1.001890272</v>
+      </c>
+      <c r="R14" t="inlineStr">
+        <is>
+          <t>2025-03-13 17:51:25</t>
+        </is>
+      </c>
+      <c r="S14" t="inlineStr">
+        <is>
+          <t>vehicle.audi.a2</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="n">
+        <v>2</v>
+      </c>
+      <c r="B15" t="n">
+        <v>10.94839857982438</v>
+      </c>
+      <c r="C15" t="n">
+        <v>0.002035810973024618</v>
+      </c>
+      <c r="D15" t="n">
+        <v>454.5780365485698</v>
+      </c>
+      <c r="E15" t="n">
+        <v>121.1400335454091</v>
+      </c>
+      <c r="F15" t="n">
+        <v>11.91579941287637</v>
+      </c>
+      <c r="G15" t="n">
+        <v>4.642350673675537</v>
+      </c>
+      <c r="H15" t="n">
+        <v>-2.196718692779541</v>
+      </c>
+      <c r="I15" t="n">
+        <v>9.721641540527344</v>
+      </c>
+      <c r="J15" t="n">
+        <v>0.005409983918070793</v>
+      </c>
+      <c r="K15" t="n">
+        <v>0.002023346722126007</v>
+      </c>
+      <c r="L15" t="n">
+        <v>-0.0826999694108963</v>
+      </c>
+      <c r="M15" t="n">
+        <v>32.07936325911004</v>
+      </c>
+      <c r="N15" t="n">
+        <v>34.78046798678554</v>
+      </c>
+      <c r="O15" t="n">
+        <v>1.993090510368347</v>
+      </c>
+      <c r="P15" t="n">
+        <v>2.706552898533774</v>
+      </c>
+      <c r="Q15" t="n">
+        <v>78.204977752</v>
+      </c>
+      <c r="R15" t="inlineStr">
+        <is>
+          <t>2025-03-13 17:52:43</t>
+        </is>
+      </c>
+      <c r="S15" t="inlineStr">
+        <is>
+          <t>vehicle.audi.a2</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="n">
+        <v>3</v>
+      </c>
+      <c r="B16" t="n">
+        <v>10.17826071375849</v>
+      </c>
+      <c r="C16" t="n">
+        <v>0.006766324397007984</v>
+      </c>
+      <c r="D16" t="n">
+        <v>441.1358654503711</v>
+      </c>
+      <c r="E16" t="n">
+        <v>128.6617263020598</v>
+      </c>
+      <c r="F16" t="n">
+        <v>6.733787362463772</v>
+      </c>
+      <c r="G16" t="n">
+        <v>-0.5927786827087402</v>
+      </c>
+      <c r="H16" t="n">
+        <v>-2.620135068893433</v>
+      </c>
+      <c r="I16" t="n">
+        <v>10.12887001037598</v>
+      </c>
+      <c r="J16" t="n">
+        <v>0.002107508946210146</v>
+      </c>
+      <c r="K16" t="n">
+        <v>-0.001142786466516554</v>
+      </c>
+      <c r="L16" t="n">
+        <v>-0.0516243688762188</v>
+      </c>
+      <c r="M16" t="n">
+        <v>32.07954763654006</v>
+      </c>
+      <c r="N16" t="n">
+        <v>34.78076612151675</v>
+      </c>
+      <c r="O16" t="n">
+        <v>2.038646697998047</v>
+      </c>
+      <c r="P16" t="n">
+        <v>2.919670128137543</v>
+      </c>
+      <c r="Q16" t="n">
+        <v>78.749327325</v>
+      </c>
+      <c r="R16" t="inlineStr">
+        <is>
+          <t>2025-03-13 17:54:02</t>
+        </is>
+      </c>
+      <c r="S16" t="inlineStr">
+        <is>
+          <t>vehicle.citroen.c3</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>